<commit_message>
Update based on new OpenAIRE data
</commit_message>
<xml_diff>
--- a/data/Manual_validation_LU_2020_2023_OpenAlex_only.xlsx
+++ b/data/Manual_validation_LU_2020_2023_OpenAlex_only.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="367" documentId="8_{22BD2A26-C1A1-4269-83E9-073ED032970D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2C93559-1BE1-4E81-8505-42213EB94CE6}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="8_{22BD2A26-C1A1-4269-83E9-073ED032970D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A56696F9-EF27-4BAC-A5B3-2A94FF83B2C2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1352FB6F-4E63-4871-BBFD-2504F0C973FF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="152">
   <si>
     <t>openalex_work_id</t>
   </si>
@@ -45,374 +45,12 @@
     <t>doi_url</t>
   </si>
   <si>
-    <t>doi_dedup___::297a19264a56d29d40642731feccc6dd</t>
-  </si>
-  <si>
-    <t>10.1371/journal.pone.0274237</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1371/journal.pone.0274237</t>
-  </si>
-  <si>
-    <t>doi_________::80a2ce26b745fad701250e2f8af66739</t>
-  </si>
-  <si>
-    <t>10.1101/2021.12.09.471697</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1101/2021.12.09.471697</t>
-  </si>
-  <si>
-    <t>doi_________::00dd5e19703c6bdb495ac93e6e9856d7</t>
-  </si>
-  <si>
-    <t>10.1101/2022.11.22.517426</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1101/2022.11.22.517426</t>
-  </si>
-  <si>
-    <t>doi_________::7c1c3b946431f0e8bed5f39440cf1bfd</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-030-95542-7_3</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-030-95542-7_3</t>
-  </si>
-  <si>
-    <t>doi_________::d6918cef9f5b3e22ac60387dde70c4dd</t>
-  </si>
-  <si>
-    <t>10.1017/9781009385084.025</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1017/9781009385084.025</t>
-  </si>
-  <si>
-    <t>doi_________::3593fa325920a45a1383664e0c117fa3</t>
-  </si>
-  <si>
-    <t>10.1017/s1743921323002521</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1017/s1743921323002521</t>
-  </si>
-  <si>
-    <t>doi_________::7ace6253a9b3932bdbdde6823dfaf5ac</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-031-29003-9_3</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-031-29003-9_3</t>
-  </si>
-  <si>
-    <t>doi_dedup___::cd8114ef089c104ddd20c09db0f77ef1</t>
-  </si>
-  <si>
-    <t>10.1016/j.bas.2021.100105</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.bas.2021.100105</t>
-  </si>
-  <si>
-    <t>doi_________::24a6f768534d520a24f77cff568952fd</t>
-  </si>
-  <si>
-    <t>10.1016/j.jcrimjus.2023.102112</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.jcrimjus.2023.102112</t>
-  </si>
-  <si>
-    <t>doi_________::f8ce217ad3f3bfe4a94bf5bcfe59a932</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-031-10370-4_1</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-031-10370-4_1</t>
-  </si>
-  <si>
-    <t>6 Leiden University Medical Center, Leiden, the Netherlands</t>
-  </si>
-  <si>
-    <t>1 Department of Anatomy and Embryology, Leiden University Medical Center, Einthovenweg 20, 2333ZC Leiden, The Netherlands
-2 Leiden Institute of Physics, Leiden University, 2333 RA, Leiden, The Netherlands
-3 Sequencing analysis support core, Leiden University Medical Center, Leiden, 2333ZA, The Netherlands</t>
-  </si>
-  <si>
-    <t>6 Faculty of Science, Leiden University, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>Institute of Environmental Sciences (CML), Leiden University, Leiden, The Netherlands</t>
-  </si>
-  <si>
     <t>Universiteit Leiden</t>
   </si>
   <si>
-    <t>5Leiden Observatory, Leiden, the Netherlands</t>
-  </si>
-  <si>
-    <t>Laboratory for Astrophysics, Leiden Observatory, Leiden University, P.O. Box 9513, 2300, RA Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>Dept of Neurosurgery, Leiden, the Netherlands</t>
-  </si>
-  <si>
-    <t>d Curium LUMC, Department of Child and Adolescent Psychiatry, Leiden University Medical Center, Leiden, the Netherlands</t>
-  </si>
-  <si>
-    <t>Leiden University, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>doi_________::25625c7337479be5392150eeb4e4546e</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-030-92087-6_33</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-030-92087-6_33</t>
-  </si>
-  <si>
-    <t>doi_________::4579462da3541a74e4e1f4ff1c138b4f</t>
-  </si>
-  <si>
-    <t>10.1136/annrheumdis-2022-eular.44</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1136/annrheumdis-2022-eular.44</t>
-  </si>
-  <si>
-    <t>doi_________::51bf102b85ddf4bdf7cf638a89d75aac</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-031-20298-8</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-031-20298-8</t>
-  </si>
-  <si>
-    <t>doi_dedup___::214498d6a97571895b7810b57282a9be</t>
-  </si>
-  <si>
-    <t>10.1038/s41409-022-01839-8</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1038/s41409-022-01839-8</t>
-  </si>
-  <si>
-    <t>doi_dedup___::a27b42cde64e387d8387ee5e5b6222c4</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-031-08601-4_1</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-031-08601-4_1</t>
-  </si>
-  <si>
-    <t>doi_________::ce63cf3c1f079c57b2653bab517f120b</t>
-  </si>
-  <si>
-    <t>10.1101/2023.11.04.565628</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1101/2023.11.04.565628</t>
-  </si>
-  <si>
-    <t>doi_________::bf0ca5ff9b73a867b578795887f9eca7</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-030-45296-4_10</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-030-45296-4_10</t>
-  </si>
-  <si>
-    <t>doi_dedup___::96bdbdddec28fe8a5790f13e03c7b8f8</t>
-  </si>
-  <si>
-    <t>10.31234/osf.io/btg8q</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.31234/osf.io/btg8q</t>
-  </si>
-  <si>
-    <t>doi_________::4ee4f9005cef66fa103408a4e04a4e4b</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-031-25248-8_5</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-031-25248-8_5</t>
-  </si>
-  <si>
-    <t>doi_________::07b9ffdde5c273c343e8352bca022111</t>
-  </si>
-  <si>
-    <t>10.1159/000535499</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1159/000535499</t>
-  </si>
-  <si>
-    <t>Department of Radiology, Leiden University Medical Center, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>9. Leiden University Medical Center, Department of Rheumatology, Leiden, Netherlands</t>
-  </si>
-  <si>
-    <t>Clinical Pharmacy and Toxicology, Leiden University Medical Center, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>15Leiden University Medical Center, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>Section of Nuclear Medicine, Department of Radiology, Leiden University Medical Center (LUMC), Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3) Department of Anatomy &amp; Embryology, Leiden University Medical Center, Leiden, Netherlands. </t>
-  </si>
-  <si>
-    <t>Department of Radiology, Section of Nuclear Medicine, Leiden University Medical Centre, Leiden, Netherlands
-Department of Radiology, Section of Nuclear Medicine and Interventional Molecular Imaging Laboratory, Leiden University Medical Center, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>1 Cognitive Psychology Unit, Institute of Psychology, Leiden University, Leiden, The Netherlands.</t>
-  </si>
-  <si>
-    <t>Parnassia Psychiatric Institute, The Hague, Leiden University &amp; University of Groningen, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>aDepartment of Pediatrics, Division of Neonatology, Willem-Alexander Children’s Hospital, Leiden University Medical Center, Leiden, The Netherlands
-bDepartment of Neurology, Leiden University Medical Center, Leiden, The Netherlands</t>
-  </si>
-  <si>
     <t>TP</t>
   </si>
   <si>
-    <t>doi_________::89635b88124925ea7e57bd53d2de98dd</t>
-  </si>
-  <si>
-    <t>10.1016/j.rpth.2023.100657</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.rpth.2023.100657</t>
-  </si>
-  <si>
-    <t>doi_dedup___::6344c46f2359f7024ed5f1320ff8642c</t>
-  </si>
-  <si>
-    <t>10.1134/s0031030123060084</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1134/s0031030123060084</t>
-  </si>
-  <si>
-    <t>doi_________::1a40dffd54e5224490aabf1c24298956</t>
-  </si>
-  <si>
-    <t>10.1007/978-94-6265-587-4</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-94-6265-587-4</t>
-  </si>
-  <si>
-    <t>doi_dedup___::d48ce85c71aec22bd69315d2b5ff4d80</t>
-  </si>
-  <si>
-    <t>10.1016/j.bas.2022.101677</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.bas.2022.101677</t>
-  </si>
-  <si>
-    <t>doi_dedup___::b83b3bb13fdfdf2c615ff932c47ba51e</t>
-  </si>
-  <si>
-    <t>10.2139/ssrn.4459559</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.2139/ssrn.4459559</t>
-  </si>
-  <si>
-    <t>doi_________::843892583a721991f504c4fbd84217ae</t>
-  </si>
-  <si>
-    <t>10.1016/j.placenta.2023.07.243</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.placenta.2023.07.243</t>
-  </si>
-  <si>
-    <t>doi_dedup___::5d5e92245a39a6313f98543d07cbe913</t>
-  </si>
-  <si>
-    <t>10.59302/ps.v100i1.13989</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.59302/ps.v100i1.13989</t>
-  </si>
-  <si>
-    <t>doi_________::8dd470f1913a465c9ca9262514a334ef</t>
-  </si>
-  <si>
-    <t>10.1017/9781108872560.014</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1017/9781108872560.014</t>
-  </si>
-  <si>
-    <t>doi_________::2e7903b29ea5bb9481c0ae9ce1492f21</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-030-97737-5_9</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/978-3-030-97737-5_9</t>
-  </si>
-  <si>
-    <t>1 Leiden University Medical Center, Leiden, Zuid-Holland, Netherlands;
-8 Department of Thrombosis and Hemostasis, Leiden University Medical Center, Leiden, The Netherlands, Leiden, Zuid-Holland, Netherlands;
-10 Department of Medicine - Thrombosis and Hemostasis, Leiden University Medical Center, Leiden, the Netherlands, Leiden, ZuidHolland, Netherlands;
-19 Leiden University Medical Center</t>
-  </si>
-  <si>
-    <t>Leiden University, 2300 RA, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>Grotius Centre for International Legal Studies, Leiden University, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>6 Department of Neurosurgery, Leiden University, Leiden, The Netherlands</t>
-  </si>
-  <si>
-    <t>Institute of Public Administration, Leiden University</t>
-  </si>
-  <si>
-    <t>2 Leiden University Medical Center, Department of Cell and Chemical Biology, Leiden, Netherlands</t>
-  </si>
-  <si>
-    <t>doi_________::48c38894ba35327fec72c47c58810961</t>
-  </si>
-  <si>
-    <t>10.1016/j.jval.2022.09.073</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.jval.2022.09.073</t>
-  </si>
-  <si>
-    <t>5Leids Universitair Medisch Centrum, Leiden, Netherlands</t>
-  </si>
-  <si>
-    <t>Eddie Denessen is bijzonder hoogleraar Sociaal-culturele achtergronden en differentiatie in het onderwijs bij het Insti-tuut Pedagogische Wetenschappen van de Universiteit Leiden (Sardesleerstoel), en universitair hoofddocent Onderwijswetenschappen van de Radboud Univer-siteit Nijmegen.</t>
-  </si>
-  <si>
-    <t>Institute for History, Leiden University, Leiden, Zuid-Holland, The Netherlands
-International Institute for Asian Studies, Leiden University, Leiden, Zuid-Holland, The Netherlands</t>
-  </si>
-  <si>
     <t>LU_affiliation_info_from_PDF_or_landing_page</t>
   </si>
   <si>
@@ -434,30 +72,6 @@
     <t>publisher</t>
   </si>
   <si>
-    <t>Abstract (conference paper) in supp/special issue</t>
-  </si>
-  <si>
-    <t>Abstract (oral communication) in supp issue</t>
-  </si>
-  <si>
-    <t>Abstract (poster) in special/supp issue</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Chapter in book</t>
-  </si>
-  <si>
-    <t>Chapter in book series</t>
-  </si>
-  <si>
-    <t>Conference paper in book series</t>
-  </si>
-  <si>
-    <t>Conference paper in proceedings</t>
-  </si>
-  <si>
     <t>Journal article</t>
   </si>
   <si>
@@ -467,55 +81,415 @@
     <t>Elsevier</t>
   </si>
   <si>
-    <t>BMJ</t>
-  </si>
-  <si>
     <t>Cambridge University Press</t>
   </si>
   <si>
     <t>Springer Nature</t>
   </si>
   <si>
-    <t>OJS</t>
-  </si>
-  <si>
     <t>SSRN</t>
   </si>
   <si>
     <t>bioRxiv</t>
   </si>
   <si>
-    <t>PsyArXiv</t>
-  </si>
-  <si>
-    <t>Karger</t>
-  </si>
-  <si>
-    <t>PLOS</t>
+    <t>other_observations</t>
+  </si>
+  <si>
+    <t>doi_________::200644765cb0789c604505852d19cf67</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-030-45296-4_16</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/978-3-030-45296-4_16</t>
+  </si>
+  <si>
+    <t>doi_dedup___::e26a7c825959ea685c9b1d4cb769b23c</t>
+  </si>
+  <si>
+    <t>10.24940/theijhss/2020/v8/i6/hs2006-082</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24940/theijhss/2020/v8/i6/hs2006-082</t>
+  </si>
+  <si>
+    <t>doi_dedup___::78e357c8aaacc473c2aee138e442bbbe</t>
+  </si>
+  <si>
+    <t>10.1016/j.jcct.2020.06.099</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jcct.2020.06.099</t>
+  </si>
+  <si>
+    <t>doi_dedup___::7f21c9e0115e5473b8d028a09a0676b2</t>
+  </si>
+  <si>
+    <t>10.1101/2023.11.21.567712</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2023.11.21.567712</t>
+  </si>
+  <si>
+    <t>doi_________::e3ed18777b24ca9b3bc0df95fa143e19</t>
+  </si>
+  <si>
+    <t>10.1136/annrheumdis-2022-eular.744</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1136/annrheumdis-2022-eular.744</t>
+  </si>
+  <si>
+    <t>doi_________::e2981761e6dbb06b0afab1437376f33f</t>
+  </si>
+  <si>
+    <t>10.1016/j.ostima.2022.100045</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ostima.2022.100045</t>
+  </si>
+  <si>
+    <t>doi_________::13f7c2f10fd4838c8fce2b0adfc12faa</t>
+  </si>
+  <si>
+    <t>10.1183/13993003.congress-2022.4139</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1183/13993003.congress-2022.4139</t>
+  </si>
+  <si>
+    <t>doi_________::23f02f3ceb827fae1e7a7329998b8bc8</t>
+  </si>
+  <si>
+    <t>10.1016/j.hpb.2022.05.325</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.hpb.2022.05.325</t>
+  </si>
+  <si>
+    <t>doi_________::39d8ae6dc01f8571d04f151e1e8d1596</t>
+  </si>
+  <si>
+    <t>10.3917/blue.001.0054</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3917/blue.001.0054</t>
+  </si>
+  <si>
+    <t>doi_dedup___::f2c37a746dd9d552d2ef0089cb47a370</t>
+  </si>
+  <si>
+    <t>10.1136/jitc-2023-sitc2023.0962</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1136/jitc-2023-sitc2023.0962</t>
+  </si>
+  <si>
+    <t>doi_________::3ea214e4664e3224f6ead8e3ae24b996</t>
+  </si>
+  <si>
+    <t>10.1681/asn.20223311s1601d</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1681/asn.20223311s1601d</t>
+  </si>
+  <si>
+    <t>doi_dedup___::447bcb08efe08182fa2c46d31e7df9df</t>
+  </si>
+  <si>
+    <t>10.1017/9781108767637.019</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/9781108767637.019</t>
+  </si>
+  <si>
+    <t>doi_dedup___::324d38a6938640f8a551015bcf565658</t>
+  </si>
+  <si>
+    <t>10.5334/cstp.459</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5334/cstp.459</t>
+  </si>
+  <si>
+    <t>doi_dedup___::fabd858267396ffa4875f14bc6df804e</t>
+  </si>
+  <si>
+    <t>10.1177/0306624x231198805</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/0306624x231198805</t>
+  </si>
+  <si>
+    <t>doi_________::88318f3da5492b4c2eb1bc591213f1aa</t>
+  </si>
+  <si>
+    <t>10.1016/j.annonc.2023.09.2857</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.annonc.2023.09.2857</t>
+  </si>
+  <si>
+    <t>doi_dedup___::25a8351e80eb8b5cc6c0a6e4a74164ec</t>
+  </si>
+  <si>
+    <t>10.1016/j.bonr.2021.101043</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.bonr.2021.101043</t>
+  </si>
+  <si>
+    <t>doi_________::6dd71df2dd8e5b76ce4e74c4535eaecc</t>
+  </si>
+  <si>
+    <t>10.1016/j.ejso.2021.12.347</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ejso.2021.12.347</t>
+  </si>
+  <si>
+    <t>doi_dedup___::f9cfa8f7d77b58df297db50f08338ab2</t>
+  </si>
+  <si>
+    <t>10.1101/2023.11.10.566569</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2023.11.10.566569</t>
+  </si>
+  <si>
+    <t>doi_________::2c1fe3b05b596df41e4f1638b7b892c3</t>
+  </si>
+  <si>
+    <t>10.47836/mjmhs.19.4.50</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.47836/mjmhs.19.4.50</t>
+  </si>
+  <si>
+    <t>doi_________::2a9a2e4507bd3d64e083fea83636ecd6</t>
+  </si>
+  <si>
+    <t>10.2139/ssrn.4280460</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2139/ssrn.4280460</t>
+  </si>
+  <si>
+    <t>doi_dedup___::c60012bb9131f2ec42805c8dbd506fbb</t>
+  </si>
+  <si>
+    <t>10.1101/2023.12.03.569402</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2023.12.03.569402</t>
+  </si>
+  <si>
+    <t>doi_________::910cd969f29a48827154b7529110fd2f</t>
+  </si>
+  <si>
+    <t>10.1017/9781108936026.006</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/9781108936026.006</t>
+  </si>
+  <si>
+    <t>doi_________::a78f4815f5cc2b97613cbb2fdf4ae67f</t>
+  </si>
+  <si>
+    <t>10.1016/j.jval.2023.03.1846</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jval.2023.03.1846</t>
+  </si>
+  <si>
+    <t>doi_dedup___::b6a355528577916446b31f0238561df6</t>
+  </si>
+  <si>
+    <t>10.48550/arxiv.2312.05351</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.48550/arxiv.2312.05351</t>
+  </si>
+  <si>
+    <t>doi_________::49c5dcf1fddd8dc52e90e1338e8bd067</t>
+  </si>
+  <si>
+    <t>10.1017/9781108647403.009</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/9781108647403.009</t>
+  </si>
+  <si>
+    <t>doi_dedup___::725df753755113b9c11d629172ddfc6e</t>
+  </si>
+  <si>
+    <t>10.48550/arxiv.2003.05759</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.48550/arxiv.2003.05759</t>
+  </si>
+  <si>
+    <t>doi_________::d009006f9dfeace70fe5399b64ee30df</t>
+  </si>
+  <si>
+    <t>10.1007/s11016-023-00944-8</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11016-023-00944-8</t>
+  </si>
+  <si>
+    <t>Abstract in special/supp issue</t>
+  </si>
+  <si>
+    <t>Book chapter</t>
+  </si>
+  <si>
+    <t>Department of Radiology, Section of Nuclear Medicine and Interventional Molecular Imaging Laboratory, Leiden University Medical Center, Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>African Studies Centre,Leiden University, Netherlands</t>
+  </si>
+  <si>
+    <t>International Journal Corner</t>
+  </si>
+  <si>
+    <t>15 Leiden University Medical Center, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>1Department of Cell and Chemical Biology, Leiden University Medical Centre, 2300 RC Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>5 Leiden University Medical Centre (LUMC), Department of Rheumatology, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎ Dept. of Rheumatology, Leiden University Medical Center, Leiden, The Netherlands &amp; Dept. of Clinical Epidemiology, Leiden University Medical Center, Leiden, The Netherlands
+⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎⁎ Leiden University, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>5 Leiden University Medical Center, Surgery, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>1 Department of Pulmonology, Leiden University Medical Center, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>European Respiratory Society</t>
+  </si>
+  <si>
+    <t>Cairn</t>
+  </si>
+  <si>
+    <t>BMJ Journals</t>
+  </si>
+  <si>
+    <t>Leiden University Medical Center, Leiden, Zuid-Holland, Netherlands</t>
+  </si>
+  <si>
+    <t>Leids Universitair Medisch Centrum, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>ASN Publications</t>
+  </si>
+  <si>
+    <t>Leiden UniversityNetherlands</t>
+  </si>
+  <si>
+    <t>Ubiquity Press</t>
+  </si>
+  <si>
+    <t>3 Department of Residential Youth Care, Leiden University of Applied Sciences and Research, The Netherlands</t>
+  </si>
+  <si>
+    <t>SAGE Publications</t>
+  </si>
+  <si>
+    <t>17 Medical Oncology Dept., Leiden University Medical Center (LUMC), Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>c Leiden University Medical Center, Department of Biomedical Data Sciences, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>7 Leiden University Medical Center, Radiation Oncology, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>3 Leiden University, Institute of Psychology and Leiden Institute for Brain and Cognition (LIBC), Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>4 Department of Anatomy and Embryology, Faculty of Medicine, Leiden University Medical Centre, 2300 RC, Leiden, The Netherlands.</t>
+  </si>
+  <si>
+    <t>Universiti Putra Malaysia</t>
+  </si>
+  <si>
+    <t>Leiden University - Health Campus The Hague
+Leiden University - Department of Clinical Epidemiology</t>
+  </si>
+  <si>
+    <t>1 Division of Systems Biomedicine and Pharmacology, LACDR, Leiden University, the Netherlands
+3 Department of Internal Medicine (Nephrology) and the Einthoven Laboratory for Vascular and Regenerative Medicine, Leiden University Medical Center (LUMC), the Netherlands</t>
+  </si>
+  <si>
+    <t>5 Leiden University Medical Center, Leiden, Netherlands</t>
+  </si>
+  <si>
+    <t>Leiden Observatory, University of Leiden, Niels Bohrweg 2, 2333 CA Leiden</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>Leiden University</t>
+  </si>
+  <si>
+    <t>Institute for History, Leiden University, Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>doi_________::11f14d629ffffe1bdd6eb803216951f9</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-030-36346-8_14</t>
+  </si>
+  <si>
+    <t>doi_dedup___::35e89c9c9acbee0ce6bde4d048c4935e</t>
+  </si>
+  <si>
+    <t>10.1101/2023.11.10.23298404</t>
+  </si>
+  <si>
+    <t>doi_dedup___::92898ea7d8f8add7ec44d0eba32ac4f8</t>
+  </si>
+  <si>
+    <t>10.1016/j.jcpa.2019.10.039</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2023.11.10.23298404</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jcpa.2019.10.039</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/978-3-030-36346-8_14</t>
+  </si>
+  <si>
+    <t>E) Leiden University Medical Center, Department of Cardiology, Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>medRxiv</t>
+  </si>
+  <si>
+    <t>‡ Anatomy &amp; Embryology, LUMC, Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>Department of Neurology, Leiden University Medical Center, Leiden, The Netherlands</t>
+  </si>
+  <si>
+    <t>Not linked to LU in OpenAIRE.</t>
+  </si>
+  <si>
+    <t>Not linked to LUMC in OpenAIRE.</t>
   </si>
   <si>
     <t>No linked organizations in OpenAIRE.</t>
-  </si>
-  <si>
-    <t>No linked organizations in OpenAIRE. Affiliation info at the end of the article.</t>
-  </si>
-  <si>
-    <t>Not linked to LU in OpenAIRE.</t>
-  </si>
-  <si>
-    <t>Not linked to LUMC in OpenAIRE.</t>
-  </si>
-  <si>
-    <t>other_observations</t>
-  </si>
-  <si>
-    <t>No linked organizations in OpenAIRE. Now linked to LU in OpenAIRE.</t>
-  </si>
-  <si>
-    <t>No linked organizations in OpenAIRE. Now linked to LUMC in OpenAIRE (but also to LU, perhaps because of Leiden University Scholarly Publications Repository).</t>
-  </si>
-  <si>
-    <t>Not linked to LUMC in OpenAIRE. Now linked to LUMC in OpenAIRE.</t>
   </si>
 </sst>
 </file>
@@ -1008,11 +982,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1389,7 +1362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5EECA6-7062-4097-AB7B-12ABE6EFADC2}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1403,18 +1376,18 @@
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61" customWidth="1"/>
+    <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.7109375" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1429,407 +1402,407 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>3213385671</v>
+        <v>4249019788</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
         <v>151</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>4388598426</v>
+        <v>3128332822</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="J3" t="s">
         <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4388608460</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>4283687153</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" t="s">
-        <v>133</v>
-      </c>
       <c r="I4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J4" t="s">
         <v>151</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>4311359186</v>
+        <v>3047262822</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>151</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4388880002</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="B6">
-        <v>4313032460</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
-      </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>4380769173</v>
+        <v>4300934281</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>151</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>4221107556</v>
+        <v>4285150194</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
         <v>151</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>2562943750</v>
+        <v>4312682199</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
         <v>151</v>
       </c>
       <c r="K9" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>4387762202</v>
+        <v>4313144073</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
         <v>151</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>4381734491</v>
+        <v>4312984006</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="J11" t="s">
         <v>151</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>4230112380</v>
+        <v>4388048412</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="J12" t="s">
         <v>151</v>
       </c>
       <c r="K12" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1837,419 +1810,419 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4312638797</v>
+        <v>2999477010</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K13" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>4327795761</v>
+        <v>4396990417</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="G14" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="J14" t="s">
         <v>151</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>4225883723</v>
+        <v>3106207538</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="J15" t="s">
         <v>151</v>
       </c>
       <c r="K15" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4281786536</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>4226468145</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" t="s">
-        <v>136</v>
-      </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="J16" t="s">
         <v>151</v>
       </c>
       <c r="K16" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>4312528293</v>
+        <v>4387661034</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G17" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>4386639548</v>
+        <v>4211209039</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="I18" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s">
         <v>151</v>
       </c>
       <c r="K18" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>4391624707</v>
+        <v>4387810188</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
         <v>151</v>
       </c>
       <c r="K19" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>4378876634</v>
+        <v>3165508775</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
         <v>151</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>4386617522</v>
+        <v>4214750940</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
         <v>102</v>
       </c>
-      <c r="F21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" t="s">
-        <v>139</v>
-      </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
         <v>151</v>
       </c>
       <c r="K21" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>4375862579</v>
+        <v>4388671234</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="I22" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>4386594982</v>
+        <v>4387754376</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
         <v>128</v>
       </c>
-      <c r="H23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" t="s">
-        <v>141</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>156</v>
+      <c r="J23" t="s">
+        <v>151</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>4390016105</v>
+        <v>4313171973</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="G24" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>157</v>
+        <v>18</v>
+      </c>
+      <c r="J24" t="s">
+        <v>151</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2257,285 +2230,334 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4389130097</v>
+        <v>4389303390</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="G25" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="J25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K25" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>4302363629</v>
+        <v>4206803704</v>
       </c>
       <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" t="s">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
       <c r="G26" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="I26" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>4303983117</v>
+        <v>4380151036</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="F27" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="I27" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K27" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>4200500391</v>
+        <v>4389649807</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="G28" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="I28" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="J28" t="s">
         <v>151</v>
       </c>
       <c r="K28" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>4309989436</v>
+        <v>4211091816</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="J29" t="s">
         <v>151</v>
       </c>
       <c r="K29" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>3160376664</v>
+        <v>3011665548</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="I30" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="J30" t="s">
         <v>151</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>4388399778</v>
+        <v>4389287003</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" t="s">
+        <v>151</v>
+      </c>
+      <c r="K31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>4211209039</v>
+      </c>
+      <c r="D40" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>4388608460</v>
+      </c>
+      <c r="D41" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>2999477010</v>
+      </c>
+      <c r="D42" t="s">
         <v>140</v>
       </c>
-      <c r="I31" t="s">
-        <v>147</v>
-      </c>
-      <c r="J31" t="s">
-        <v>154</v>
-      </c>
-      <c r="K31" t="s">
-        <v>84</v>
+      <c r="E42" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K31" xr:uid="{DC5EECA6-7062-4097-AB7B-12ABE6EFADC2}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
-      <sortCondition ref="G2:G31"/>
-      <sortCondition ref="H2:H31"/>
-      <sortCondition ref="J2:J31"/>
+      <sortCondition ref="A1:A31"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E26" r:id="rId1" xr:uid="{D9C1E61E-5D9C-4FA0-940A-FC0621A7FCD2}"/>
-    <hyperlink ref="E28" r:id="rId2" xr:uid="{068A707B-5164-44B5-9213-CA145B3B4196}"/>
-    <hyperlink ref="E29" r:id="rId3" xr:uid="{25921A2E-19EA-4AB8-B297-E167F33F436D}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{82B70CC5-5AFC-4B3D-B356-0F3D7278BC68}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{9E444744-D9AA-4F66-B44E-A3869942A07C}"/>
-    <hyperlink ref="E19" r:id="rId6" xr:uid="{F279644F-A53D-4647-AF01-089ED2D73A61}"/>
-    <hyperlink ref="E18" r:id="rId7" xr:uid="{D3B3A7E1-0E34-429F-A5A6-12E4CAF32193}"/>
-    <hyperlink ref="E2" r:id="rId8" xr:uid="{2CCA53DC-FE0A-405F-B1F1-F2B8AB39D71C}"/>
-    <hyperlink ref="E23" r:id="rId9" xr:uid="{5C0B4D34-2782-4EA3-815D-6156D8BC2A75}"/>
-    <hyperlink ref="E14" r:id="rId10" xr:uid="{B66BD5FF-0479-4984-B22F-92F48EDD1632}"/>
-    <hyperlink ref="E16" r:id="rId11" xr:uid="{282A8836-D8F2-474F-B2F8-D177B6E0F82E}"/>
-    <hyperlink ref="E4" r:id="rId12" xr:uid="{5A1C317F-2118-4F7B-8200-9F1CC856C9BA}"/>
-    <hyperlink ref="E7" r:id="rId13" xr:uid="{C028BDE9-D599-4B3F-88B3-8849B95FF755}"/>
-    <hyperlink ref="E27" r:id="rId14" xr:uid="{A947E6A7-3DBD-4B06-B1B9-0FA7F56432D1}"/>
-    <hyperlink ref="E13" r:id="rId15" xr:uid="{E0250491-7753-4EF0-B6CA-4E2D325C86C2}"/>
-    <hyperlink ref="E31" r:id="rId16" xr:uid="{2D9E2DD8-F281-4E00-A835-381C7E77C8FA}"/>
-    <hyperlink ref="E12" r:id="rId17" xr:uid="{6B7A57E5-9683-46D7-9E6B-C51374A35FBF}"/>
-    <hyperlink ref="E30" r:id="rId18" xr:uid="{65534CAF-BC15-489F-87BA-C0FAFD60D755}"/>
-    <hyperlink ref="E11" r:id="rId19" xr:uid="{A79AA860-2C7C-413D-8A00-897CD5525042}"/>
-    <hyperlink ref="E24" r:id="rId20" xr:uid="{D9A4A5DD-B61A-428E-87A2-CA03EC0300B4}"/>
-    <hyperlink ref="E3" r:id="rId21" xr:uid="{59E0D205-3F8F-49F9-9E45-03F86D567BE6}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{3DFB464E-F41E-4CDF-80FF-798705703487}"/>
-    <hyperlink ref="E9" r:id="rId23" xr:uid="{62DB4264-2EC1-43E3-BA5A-F8561F6783FC}"/>
-    <hyperlink ref="E6" r:id="rId24" xr:uid="{3A3416F6-03CF-4939-93C1-3D6F24643E92}"/>
-    <hyperlink ref="E20" r:id="rId25" xr:uid="{57A51C3C-3A69-4ED1-A39D-A608202AD4BF}"/>
-    <hyperlink ref="E21" r:id="rId26" xr:uid="{9580D5A3-38F2-45DC-81CC-313C88DBC111}"/>
-    <hyperlink ref="E5" r:id="rId27" xr:uid="{14E1F085-E041-4CD4-A308-8CC5D1993085}"/>
-    <hyperlink ref="E22" r:id="rId28" xr:uid="{6C1EB7EA-F350-4838-96C6-D7EF64FD4986}"/>
-    <hyperlink ref="E8" r:id="rId29" xr:uid="{1DA92416-04FE-46D1-B651-3FFA2BDF9F12}"/>
-    <hyperlink ref="E17" r:id="rId30" xr:uid="{743B7E5A-D378-496C-9829-3326374D0EA9}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{0DD3419E-E47D-49D3-9131-D85A5C572208}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{53F2EB89-59FD-44A0-8AF5-5B2D982A8E6C}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{80D179B7-40AA-4DE5-9B1E-383841AB8AB2}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{4E9B13D4-CD8F-42A4-A2D3-8307CD989A78}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{C058AE9A-51D7-4E21-BE4F-55DF9D5BFBC5}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{5421664D-BC4C-48CE-AAA9-709406B0791B}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{0704594D-2EB0-4B81-901F-98697A516121}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{68E820EE-87E2-454D-AF97-B9D318B11035}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{861AC3DA-C2F4-459F-A273-145A58B94A11}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{D9C70AB2-0E9C-4767-BD77-214E2BF145EF}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{F97DC84C-EB60-4571-B0E0-91C9FF925EDC}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{F3A1FCA5-064F-49FD-B4CE-FE152579B2D0}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{59C71D5E-BF52-41FA-B280-939511144D69}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{D36231AD-7C17-48E2-A9C0-C6BDDD0E5B8B}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{984F51C9-27DD-4648-A7F7-5BC7E115DDA4}"/>
+    <hyperlink ref="E20" r:id="rId16" xr:uid="{37F9203A-7035-40C3-B29F-51F70CCE2246}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{852C4EFA-CE54-4161-86FE-098A41696262}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{1F2FC09A-BBAF-4581-A6B2-A3BAB13B3E42}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{61098939-298E-4F08-B7F0-077395FAFB2F}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{18371B64-4419-4112-A2EB-5D52015147E8}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{0CB20DD3-A30E-4CAF-B37E-89B6BEEE7823}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{D9C0DB7A-A551-4D41-AC3D-2DBB1144E9CC}"/>
+    <hyperlink ref="E27" r:id="rId23" xr:uid="{EFBB4153-86AD-4F15-94EB-C6DE046DAAB7}"/>
+    <hyperlink ref="E28" r:id="rId24" xr:uid="{0DD7364B-D63A-4C16-935E-A34B355F4A0D}"/>
+    <hyperlink ref="E29" r:id="rId25" xr:uid="{99624CDA-EA6C-4BF9-A089-4ABE9C7EE773}"/>
+    <hyperlink ref="E30" r:id="rId26" xr:uid="{97753DFA-79EB-48FD-BD54-4B7003F11E11}"/>
+    <hyperlink ref="E31" r:id="rId27" xr:uid="{7DD54C8C-25E7-4D0F-BFD8-56341140D74C}"/>
+    <hyperlink ref="E4" r:id="rId28" xr:uid="{9930BA57-F20F-4441-94B3-9A0118A37447}"/>
+    <hyperlink ref="E13" r:id="rId29" xr:uid="{C06CB092-BAF4-47C9-8A03-121A4229351E}"/>
+    <hyperlink ref="E18" r:id="rId30" xr:uid="{38DC8002-C4AA-4D35-B2FC-2A7533CA4867}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId31"/>

</xml_diff>